<commit_message>
user Mgmt Data and Business layers completed.
</commit_message>
<xml_diff>
--- a/dev_support/log_messages.xlsx
+++ b/dev_support/log_messages.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstrobel/Dropbox/Develop/Projekte/haushalt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rstrobel/Dropbox/Develop/Projekte/haushalt/dev_support/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>'CRITICAL', 1000, __name__, 'Error getting db connect parameters.'</t>
   </si>
@@ -113,7 +113,16 @@
     <t>'DEBUG', 1203, __name__, 'Log_format:' + log_format</t>
   </si>
   <si>
-    <t>lib_usr (2000 - 2999)</t>
+    <t>lib_usr_bl (2200 - 2399)</t>
+  </si>
+  <si>
+    <t>lib_usr_dl (2000 - 2199)</t>
+  </si>
+  <si>
+    <t>lib_usr_pl (2400 - 2599)</t>
+  </si>
+  <si>
+    <t>WARNING', 2201, __name__, 'Error selecting user.'</t>
   </si>
 </sst>
 </file>
@@ -178,10 +187,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,11 +493,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -521,11 +530,11 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
@@ -547,7 +556,7 @@
         <f>LEFT(C11,SEARCH(",",C11,1)-1)</f>
         <v>CRITICAL'</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -619,7 +628,7 @@
         <f t="shared" si="0"/>
         <v>CRITICAL'</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -636,18 +645,18 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
@@ -657,7 +666,7 @@
         <f t="shared" ref="B24:B27" si="1">LEFT(C24,SEARCH(",",C24,1)-1)</f>
         <v>'INFO'</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -669,7 +678,7 @@
         <f t="shared" si="1"/>
         <v>'INFO'</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -681,7 +690,7 @@
         <f t="shared" si="1"/>
         <v>'INFO'</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -693,16 +702,16 @@
         <f t="shared" si="1"/>
         <v>'DEBUG'</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="A33" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
@@ -820,63 +829,29 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="4">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="4">
-        <v>3001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="4">
-        <v>3002</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="4">
-        <v>3003</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="4">
-        <v>3004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="4">
-        <v>3005</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="4">
-        <v>3006</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="4">
-        <v>3007</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="4">
-        <v>3008</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4">
-        <v>3009</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="4">
-        <v>3010</v>
-      </c>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C47" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A57:C57"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A20:C20"/>

</xml_diff>